<commit_message>
worked on admin sub admin , lead assignment, and mobile view and also severl backend
</commit_message>
<xml_diff>
--- a/backend/public/lead-bulk-template.xlsx
+++ b/backend/public/lead-bulk-template.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>name</t>
   </si>
@@ -23,6 +23,9 @@
   </si>
   <si>
     <t>budget</t>
+  </si>
+  <si>
+    <t>propertyType</t>
   </si>
   <si>
     <t>flatType</t>
@@ -414,18 +417,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:H1"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="25" customWidth="1"/>
     <col min="2" max="2" width="20" style="1" customWidth="1"/>
     <col min="3" max="3" width="20" customWidth="1"/>
-    <col min="4" max="5" width="15" customWidth="1"/>
-    <col min="6" max="6" width="25" customWidth="1"/>
-    <col min="7" max="7" width="30" customWidth="1"/>
+    <col min="4" max="4" width="15" customWidth="1"/>
+    <col min="5" max="5" width="20" customWidth="1"/>
+    <col min="6" max="6" width="15" customWidth="1"/>
+    <col min="7" max="7" width="25" customWidth="1"/>
+    <col min="8" max="8" width="30" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -447,16 +452,22 @@
       <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
   </sheetData>
-  <dataValidations count="3">
+  <dataValidations count="4">
     <dataValidation type="list" allowBlank="1" sqref="D2:D5000">
       <formula1>"0-10000,10000-20000,20000-30000,30000-50000,50000-75000,75000-100000,100000-above"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" sqref="E2:E5000">
+      <formula1>"Standalone house,Apartment,Gated community,Independent house,Villa,PG / Co-living,Plot / Land"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" sqref="F2:F5000">
       <formula1>"1RK,1BHK,2BHK,3BHK,4BHK,Villa,Penthouse"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="F2:F5000">
+    <dataValidation type="list" allowBlank="1" sqref="G2:G5000">
       <formula1>"Whitefield,Indiranagar,Koramangala,Bengaluru,Jayanagar,Banashankari,Basaveshwaranagar,Bheemanahalli,Bommanahalli,Chikkalasandra,Dasarahalli,Domlur,Electronic City,Frazer Town,Girinagar,Gokula,Gopalapuram,Hanumanthanagar,HBR Layout,Hebbal,Hoysala,HSR Layout,Ittamadu,JP Nagar,Jyothinagar,Kammanahalli,Kaval Byrasandra,Kodichikkanahalli,Kommadi,Kundalahalli,Lingrajapuram,Mahadevapura,Malleswaram,Marathahalli,Mathikere,Mico Layout,Mookambika,Nagavara,Nagawara,Nagarathpet,Nandini Layout,Nayandahalli,Old Airport Road,Peenya,Prithviraj Road,RMV Extension,Sadashivnagar,Sahakarnagar,Sanjaynagar,Sarjapur Road,Seshadripuram,Shantinagar,Shivaji Nagar,Soladevanahalli,Subramanyanagar"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
changes in lead and broker
</commit_message>
<xml_diff>
--- a/backend/public/lead-bulk-template.xlsx
+++ b/backend/public/lead-bulk-template.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>name</t>
   </si>
@@ -29,6 +29,12 @@
   </si>
   <si>
     <t>flatType</t>
+  </si>
+  <si>
+    <t>furnishingType</t>
+  </si>
+  <si>
+    <t>amenities</t>
   </si>
   <si>
     <t>areaKey</t>
@@ -417,20 +423,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:J1"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="25" customWidth="1"/>
     <col min="2" max="2" width="20" style="1" customWidth="1"/>
-    <col min="3" max="3" width="20" customWidth="1"/>
-    <col min="4" max="4" width="15" customWidth="1"/>
-    <col min="5" max="5" width="20" customWidth="1"/>
-    <col min="6" max="6" width="15" customWidth="1"/>
-    <col min="7" max="7" width="25" customWidth="1"/>
+    <col min="3" max="3" width="25" customWidth="1"/>
+    <col min="4" max="4" width="18" customWidth="1"/>
+    <col min="5" max="5" width="22" customWidth="1"/>
+    <col min="6" max="6" width="18" customWidth="1"/>
+    <col min="7" max="7" width="20" customWidth="1"/>
     <col min="8" max="8" width="30" customWidth="1"/>
+    <col min="9" max="9" width="25" customWidth="1"/>
+    <col min="10" max="10" width="30" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -455,19 +463,31 @@
       <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
     </row>
   </sheetData>
-  <dataValidations count="4">
+  <dataValidations count="6">
     <dataValidation type="list" allowBlank="1" sqref="D2:D5000">
-      <formula1>"0-10000,10000-20000,20000-30000,30000-50000,50000-75000,75000-100000,100000-above"</formula1>
+      <formula1>"10000-15000,15000-20000,20000-25000,25000-35000,35000-50000,50000-above"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" sqref="E2:E5000">
-      <formula1>"Standalone house,Apartment,Gated community,Independent house,Villa,PG / Co-living,Plot / Land"</formula1>
+      <formula1>"Standalone house,Apartment,Gated community,Independent house,Villa,PG / Co-living,Plot / Land,Anything is fine"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" sqref="F2:F5000">
-      <formula1>"1RK,1BHK,2BHK,3BHK,4BHK,Villa,Penthouse"</formula1>
+      <formula1>"1RK,1BHK,2BHK,3BHK,4BHK,Villa,Penthouse,Anything is fine"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" sqref="G2:G5000">
+      <formula1>"Fully Furnished,Semi Furnished,Unfurnished"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" sqref="H2:H5000">
+      <formula1>"Parking,Security,Power backup,Lift,Balcony"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" sqref="I2:I5000">
       <formula1>"Whitefield,Indiranagar,Koramangala,Bengaluru,Jayanagar,Banashankari,Basaveshwaranagar,Bheemanahalli,Bommanahalli,Chikkalasandra,Dasarahalli,Domlur,Electronic City,Frazer Town,Girinagar,Gokula,Gopalapuram,Hanumanthanagar,HBR Layout,Hebbal,Hoysala,HSR Layout,Ittamadu,JP Nagar,Jyothinagar,Kammanahalli,Kaval Byrasandra,Kodichikkanahalli,Kommadi,Kundalahalli,Lingrajapuram,Mahadevapura,Malleswaram,Marathahalli,Mathikere,Mico Layout,Mookambika,Nagavara,Nagawara,Nagarathpet,Nandini Layout,Nayandahalli,Old Airport Road,Peenya,Prithviraj Road,RMV Extension,Sadashivnagar,Sahakarnagar,Sanjaynagar,Sarjapur Road,Seshadripuram,Shantinagar,Shivaji Nagar,Soladevanahalli,Subramanyanagar"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>